<commit_message>
Ajout des planetes dans le graphique
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="50">
   <si>
     <t>Condition initiales de la simulation</t>
   </si>
@@ -159,13 +159,28 @@
   </si>
   <si>
     <t>qk</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Vars for planet 1</t>
+  </si>
+  <si>
+    <t>angle</t>
+  </si>
+  <si>
+    <t>Vars for planet 2</t>
+  </si>
+  <si>
+    <t>Vars for planet 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,14 +204,6 @@
     </font>
     <font>
       <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -442,7 +449,7 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -519,9 +526,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -616,87 +620,94 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="20 % - Accent1" xfId="2" builtinId="30"/>
@@ -739,6 +750,35 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-CA"/>
+              <a:t>Systeme</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-CA" baseline="0"/>
+              <a:t> Solaire</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -778,6 +818,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$B$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Corp 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -788,31 +839,100 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$T$6:$T$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24330.127018922194</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15669.872981077806</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15669.872981077806</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17499.999999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24330.12701892219</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$D$18:$E$18</c:f>
+              <c:f>Feuil1!$U$6:$U$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>20000</c:v>
+                  <c:v>7500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7500</c:v>
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11830.127018922194</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11830.127018922194</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7500.0000000000009</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5000.0000000000018</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3169.8729810778077</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3169.8729810778068</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4999.9999999999982</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7499.9999999999991</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -820,7 +940,265 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-CCE0-45C9-A600-6E11F7FB8C7A}"/>
+              <c16:uniqueId val="{00000000-D3E0-4743-8C92-751DDA7B01B5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$B$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Corps 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$W$6:$W$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>-16500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-16968.911086754466</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-18250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-20000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-21750</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-23031.088913245534</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-23500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-23031.088913245534</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-21750</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-20000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-18250</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-16968.911086754466</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-16500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$X$6:$X$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11750</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13031.088913245534</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13031.088913245536</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11750</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8250</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6968.9110867544659</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6968.911086754465</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8249.9999999999982</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D3E0-4743-8C92-751DDA7B01B5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$B$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Corps 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$Z$6:$Z$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-669.8729810778068</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2499.9999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-5000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-7499.9999999999991</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-9330.1270189221941</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-10000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-9330.1270189221941</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-7500.0000000000018</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-5000.0000000000009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-2499.9999999999995</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-669.87298107780771</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$AA$6:$AA$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>-15000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-12500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-10669.872981077806</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-10669.872981077806</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-12500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-15000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-17500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-19330.12701892219</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-20000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-19330.127018922194</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-17500.000000000004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-15000.000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D3E0-4743-8C92-751DDA7B01B5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -832,11 +1210,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2028194640"/>
-        <c:axId val="2028193808"/>
+        <c:axId val="1217205519"/>
+        <c:axId val="1244306047"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2028194640"/>
+        <c:axId val="1217205519"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -856,6 +1234,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -892,12 +1271,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2028193808"/>
+        <c:crossAx val="1244306047"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2028193808"/>
+        <c:axId val="1244306047"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -954,7 +1333,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2028194640"/>
+        <c:crossAx val="1217205519"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1564,19 +1943,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>8657</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>13853</xdr:rowOff>
+      <xdr:colOff>299356</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>43545</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>363680</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>40821</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>17316</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Graphique 2"/>
+        <xdr:cNvPr id="4" name="Graphique 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1857,10 +2236,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O42"/>
+  <dimension ref="B2:AA42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U28" sqref="U28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1869,113 +2248,297 @@
     <col min="3" max="3" width="7.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" customWidth="1"/>
     <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71" t="s">
+    <row r="2" spans="2:27" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="71" t="s">
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-    </row>
-    <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
+    </row>
+    <row r="3" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W3" s="99"/>
+      <c r="X3" s="99"/>
+      <c r="Y3" s="99"/>
+    </row>
+    <row r="4" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="38"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="26"/>
-      <c r="E4" s="39"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T4" s="97" t="s">
+        <v>46</v>
+      </c>
+      <c r="U4" s="97"/>
+      <c r="W4" s="97" t="s">
+        <v>48</v>
+      </c>
+      <c r="X4" s="97"/>
+      <c r="Z4" s="97" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA4" s="97"/>
+    </row>
+    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="76">
+      <c r="D5" s="93">
         <v>0.5</v>
       </c>
-      <c r="E5" s="77"/>
-      <c r="F5" s="53" t="s">
+      <c r="E5" s="94"/>
+      <c r="F5" s="52" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="R5" t="s">
+        <v>47</v>
+      </c>
+      <c r="T5" t="s">
+        <v>45</v>
+      </c>
+      <c r="U5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="98" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="76">
+      <c r="D6" s="93">
         <v>0</v>
       </c>
-      <c r="E6" s="77"/>
-      <c r="F6" s="53" t="s">
+      <c r="E6" s="94"/>
+      <c r="F6" s="52" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <f>Q6*(2*PI())/12</f>
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <f>(COS(R6)*$D$19)+$D$18</f>
+        <v>25000</v>
+      </c>
+      <c r="U6">
+        <f>(SIN(R6)*$D$19)+$E$18</f>
+        <v>7500</v>
+      </c>
+      <c r="W6">
+        <f>(COS(R6)*$D$28)+$D$27</f>
+        <v>-16500</v>
+      </c>
+      <c r="X6">
+        <f>(SIN(R6)*$D$28)+$E$27</f>
+        <v>10000</v>
+      </c>
+      <c r="Z6">
+        <f>(COS(R6)*$D$37)+$D$36</f>
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <f>(SIN(R6)*$D$37)+$E$36</f>
+        <v>-15000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="78">
+      <c r="D7" s="95">
         <v>1</v>
       </c>
-      <c r="E7" s="79"/>
-      <c r="F7" s="54" t="s">
+      <c r="E7" s="96"/>
+      <c r="F7" s="53" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q7">
+        <f>Q6+1</f>
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <f t="shared" ref="R7:R18" si="0">Q7*(2*PI())/12</f>
+        <v>0.52359877559829882</v>
+      </c>
+      <c r="T7">
+        <f t="shared" ref="T7:T18" si="1">(COS(R7)*$D$19)+$D$18</f>
+        <v>24330.127018922194</v>
+      </c>
+      <c r="U7">
+        <f t="shared" ref="U7:U18" si="2">(SIN(R7)*$D$19)+$E$18</f>
+        <v>10000</v>
+      </c>
+      <c r="W7">
+        <f t="shared" ref="W7:W18" si="3">(COS(R7)*$D$28)+$D$27</f>
+        <v>-16968.911086754466</v>
+      </c>
+      <c r="X7">
+        <f t="shared" ref="X7:X18" si="4">(SIN(R7)*$D$28)+$E$27</f>
+        <v>11750</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" ref="Z7:Z18" si="5">(COS(R7)*$D$37)+$D$36</f>
+        <v>-669.8729810778068</v>
+      </c>
+      <c r="AA7">
+        <f t="shared" ref="AA7:AA18" si="6">(SIN(R7)*$D$37)+$E$36</f>
+        <v>-12500</v>
+      </c>
+    </row>
+    <row r="8" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
-      <c r="F8" s="50"/>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F8" s="49"/>
+      <c r="Q8">
+        <f t="shared" ref="Q8:Q18" si="7">Q7+1</f>
+        <v>2</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="0"/>
+        <v>1.0471975511965976</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="1"/>
+        <v>22500</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="2"/>
+        <v>11830.127018922194</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="3"/>
+        <v>-18250</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="4"/>
+        <v>13031.088913245534</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="5"/>
+        <v>-2499.9999999999995</v>
+      </c>
+      <c r="AA8">
+        <f t="shared" si="6"/>
+        <v>-10669.872981077806</v>
+      </c>
+    </row>
+    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
       <c r="E9" s="31"/>
-      <c r="F9" s="55"/>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F9" s="54"/>
+      <c r="Q9">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="0"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="1"/>
+        <v>20000</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="2"/>
+        <v>12500</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="3"/>
+        <v>-20000</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="4"/>
+        <v>13500</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="5"/>
+        <v>-5000</v>
+      </c>
+      <c r="AA9">
+        <f t="shared" si="6"/>
+        <v>-10000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="72">
+      <c r="D10" s="89">
         <v>1</v>
       </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="67" t="s">
+      <c r="E10" s="90"/>
+      <c r="F10" s="66" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q10">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="0"/>
+        <v>2.0943951023931953</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="1"/>
+        <v>17500</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="2"/>
+        <v>11830.127018922194</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="3"/>
+        <v>-21750</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="4"/>
+        <v>13031.088913245536</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="5"/>
+        <v>-7499.9999999999991</v>
+      </c>
+      <c r="AA10">
+        <f t="shared" si="6"/>
+        <v>-10669.872981077806</v>
+      </c>
+    </row>
+    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>7</v>
       </c>
@@ -1988,11 +2551,43 @@
       <c r="E11" s="17">
         <v>0</v>
       </c>
-      <c r="F11" s="51" t="s">
+      <c r="F11" s="50" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q11">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="0"/>
+        <v>2.6179938779914944</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="1"/>
+        <v>15669.872981077806</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="2"/>
+        <v>10000</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="3"/>
+        <v>-23031.088913245534</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="4"/>
+        <v>11750</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="5"/>
+        <v>-9330.1270189221941</v>
+      </c>
+      <c r="AA11">
+        <f t="shared" si="6"/>
+        <v>-12500</v>
+      </c>
+    </row>
+    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>8</v>
       </c>
@@ -2005,11 +2600,43 @@
       <c r="E12" s="17">
         <v>0</v>
       </c>
-      <c r="F12" s="51" t="s">
+      <c r="F12" s="50" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q12">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="0"/>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="1"/>
+        <v>15000</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="2"/>
+        <v>7500.0000000000009</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="3"/>
+        <v>-23500</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="4"/>
+        <v>10000</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="5"/>
+        <v>-10000</v>
+      </c>
+      <c r="AA12">
+        <f t="shared" si="6"/>
+        <v>-15000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>9</v>
       </c>
@@ -2022,165 +2649,357 @@
       <c r="E13" s="17">
         <v>0</v>
       </c>
-      <c r="F13" s="51" t="s">
+      <c r="F13" s="50" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q13">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="0"/>
+        <v>3.6651914291880918</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="1"/>
+        <v>15669.872981077806</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="2"/>
+        <v>5000.0000000000018</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="3"/>
+        <v>-23031.088913245534</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="4"/>
+        <v>8250</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="5"/>
+        <v>-9330.1270189221941</v>
+      </c>
+      <c r="AA13">
+        <f t="shared" si="6"/>
+        <v>-17500</v>
+      </c>
+    </row>
+    <row r="14" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="74">
+      <c r="D14" s="91">
         <v>2500</v>
       </c>
-      <c r="E14" s="75"/>
-      <c r="F14" s="52" t="s">
+      <c r="E14" s="92"/>
+      <c r="F14" s="51" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q14">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="0"/>
+        <v>4.1887902047863905</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="1"/>
+        <v>17499.999999999996</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="2"/>
+        <v>3169.8729810778077</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="3"/>
+        <v>-21750</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="4"/>
+        <v>6968.9110867544659</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="5"/>
+        <v>-7500.0000000000018</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" si="6"/>
+        <v>-19330.12701892219</v>
+      </c>
+    </row>
+    <row r="15" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="1"/>
-      <c r="F15" s="50"/>
-    </row>
-    <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="49"/>
+      <c r="Q15">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="0"/>
+        <v>4.7123889803846897</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="1"/>
+        <v>20000</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="2"/>
+        <v>2500</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="3"/>
+        <v>-20000</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="4"/>
+        <v>6500</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="5"/>
+        <v>-5000.0000000000009</v>
+      </c>
+      <c r="AA15">
+        <f t="shared" si="6"/>
+        <v>-20000</v>
+      </c>
+    </row>
+    <row r="16" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="34"/>
       <c r="D16" s="34"/>
       <c r="E16" s="34"/>
-      <c r="F16" s="56"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="55"/>
+      <c r="Q16">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="0"/>
+        <v>5.2359877559829888</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="1"/>
+        <v>22500</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="2"/>
+        <v>3169.8729810778068</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="3"/>
+        <v>-18250</v>
+      </c>
+      <c r="X16">
+        <f t="shared" si="4"/>
+        <v>6968.911086754465</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" si="5"/>
+        <v>-2499.9999999999995</v>
+      </c>
+      <c r="AA16">
+        <f t="shared" si="6"/>
+        <v>-19330.127018922194</v>
+      </c>
+    </row>
+    <row r="17" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B17" s="27" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="11"/>
-      <c r="D17" s="80"/>
-      <c r="E17" s="80"/>
-      <c r="F17" s="57"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="56"/>
+      <c r="Q17">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="0"/>
+        <v>5.7595865315812871</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="1"/>
+        <v>24330.12701892219</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="2"/>
+        <v>4999.9999999999982</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="3"/>
+        <v>-16968.911086754466</v>
+      </c>
+      <c r="X17">
+        <f t="shared" si="4"/>
+        <v>8249.9999999999982</v>
+      </c>
+      <c r="Z17">
+        <f t="shared" si="5"/>
+        <v>-669.87298107780771</v>
+      </c>
+      <c r="AA17">
+        <f t="shared" si="6"/>
+        <v>-17500.000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B18" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="88" t="s">
+      <c r="C18" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="86">
+      <c r="D18" s="72">
         <v>20000</v>
       </c>
-      <c r="E18" s="87">
+      <c r="E18" s="73">
         <v>7500</v>
       </c>
-      <c r="F18" s="70" t="s">
+      <c r="F18" s="69" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="Q18">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="0"/>
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="1"/>
+        <v>25000</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="2"/>
+        <v>7499.9999999999991</v>
+      </c>
+      <c r="W18">
+        <f t="shared" si="3"/>
+        <v>-16500</v>
+      </c>
+      <c r="X18">
+        <f t="shared" si="4"/>
+        <v>10000</v>
+      </c>
+      <c r="Z18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AA18">
+        <f t="shared" si="6"/>
+        <v>-15000.000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B19" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="88" t="s">
+      <c r="C19" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="81">
+      <c r="D19" s="85">
         <v>5000</v>
       </c>
-      <c r="E19" s="82"/>
-      <c r="F19" s="70" t="s">
+      <c r="E19" s="86"/>
+      <c r="F19" s="69" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B20" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="88" t="s">
+      <c r="C20" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="81">
+      <c r="D20" s="85">
         <v>1</v>
       </c>
-      <c r="E20" s="82"/>
-      <c r="F20" s="70" t="s">
+      <c r="E20" s="86"/>
+      <c r="F20" s="69" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B21" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="88" t="s">
+      <c r="C21" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="83"/>
-      <c r="E21" s="83"/>
-      <c r="F21" s="70" t="s">
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="69" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B22" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="88" t="s">
+      <c r="C22" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="83"/>
-      <c r="E22" s="83"/>
-      <c r="F22" s="70" t="s">
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="69" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B23" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="88" t="s">
+      <c r="C23" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="83"/>
-      <c r="E23" s="83"/>
-      <c r="F23" s="70" t="s">
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="69" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="89" t="s">
+      <c r="C24" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="84" t="s">
+      <c r="D24" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="85"/>
-      <c r="F24" s="69" t="s">
+      <c r="E24" s="88"/>
+      <c r="F24" s="68" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="29"/>
       <c r="C25" s="30"/>
       <c r="D25" s="30"/>
       <c r="E25" s="30"/>
-      <c r="F25" s="58"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="40" t="s">
+      <c r="F25" s="57"/>
+    </row>
+    <row r="26" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B26" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="42"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="59"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C26" s="41"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="58"/>
+    </row>
+    <row r="27" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>13</v>
       </c>
@@ -2193,41 +3012,41 @@
       <c r="E27" s="22">
         <v>10000</v>
       </c>
-      <c r="F27" s="60" t="s">
+      <c r="F27" s="59" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="90">
+      <c r="D28" s="76">
         <v>3500</v>
       </c>
-      <c r="E28" s="91"/>
-      <c r="F28" s="61" t="s">
+      <c r="E28" s="77"/>
+      <c r="F28" s="60" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="90">
+      <c r="D29" s="76">
         <v>1</v>
       </c>
-      <c r="E29" s="91"/>
-      <c r="F29" s="61" t="s">
+      <c r="E29" s="77"/>
+      <c r="F29" s="60" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>16</v>
       </c>
@@ -2236,11 +3055,11 @@
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="23"/>
-      <c r="F30" s="61" t="s">
+      <c r="F30" s="60" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>17</v>
       </c>
@@ -2249,11 +3068,11 @@
       </c>
       <c r="D31" s="21"/>
       <c r="E31" s="23"/>
-      <c r="F31" s="61" t="s">
+      <c r="F31" s="60" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>18</v>
       </c>
@@ -2262,22 +3081,22 @@
       </c>
       <c r="D32" s="21"/>
       <c r="E32" s="23"/>
-      <c r="F32" s="61" t="s">
+      <c r="F32" s="60" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="41" t="s">
+      <c r="B33" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="43" t="s">
+      <c r="C33" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="D33" s="92" t="s">
+      <c r="D33" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="E33" s="93"/>
-      <c r="F33" s="62" t="s">
+      <c r="E33" s="79"/>
+      <c r="F33" s="61" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2286,16 +3105,16 @@
       <c r="C34" s="30"/>
       <c r="D34" s="30"/>
       <c r="E34" s="30"/>
-      <c r="F34" s="63"/>
+      <c r="F34" s="62"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="46" t="s">
+      <c r="B35" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="47"/>
-      <c r="D35" s="48"/>
-      <c r="E35" s="49"/>
-      <c r="F35" s="64"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="48"/>
+      <c r="F35" s="63"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
@@ -2310,7 +3129,7 @@
       <c r="E36" s="25">
         <v>-15000</v>
       </c>
-      <c r="F36" s="65" t="s">
+      <c r="F36" s="64" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2321,11 +3140,11 @@
       <c r="C37" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D37" s="96">
+      <c r="D37" s="82">
         <v>5000</v>
       </c>
-      <c r="E37" s="97"/>
-      <c r="F37" s="65" t="s">
+      <c r="E37" s="83"/>
+      <c r="F37" s="64" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2336,11 +3155,11 @@
       <c r="C38" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D38" s="96">
+      <c r="D38" s="82">
         <v>1</v>
       </c>
-      <c r="E38" s="97"/>
-      <c r="F38" s="65" t="s">
+      <c r="E38" s="83"/>
+      <c r="F38" s="64" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2353,7 +3172,7 @@
       </c>
       <c r="D39" s="24"/>
       <c r="E39" s="25"/>
-      <c r="F39" s="65" t="s">
+      <c r="F39" s="64" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2366,7 +3185,7 @@
       </c>
       <c r="D40" s="24"/>
       <c r="E40" s="25"/>
-      <c r="F40" s="65" t="s">
+      <c r="F40" s="64" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2379,7 +3198,7 @@
       </c>
       <c r="D41" s="24"/>
       <c r="E41" s="25"/>
-      <c r="F41" s="65" t="s">
+      <c r="F41" s="64" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2390,22 +3209,19 @@
       <c r="C42" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D42" s="94" t="s">
+      <c r="D42" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="E42" s="95"/>
-      <c r="F42" s="66" t="s">
+      <c r="E42" s="81"/>
+      <c r="F42" s="65" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
+  <mergeCells count="19">
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="Z4:AA4"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D20:E20"/>
@@ -2416,6 +3232,12 @@
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ajout des valeurs manquantes
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -449,7 +449,7 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -493,13 +493,7 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
@@ -623,9 +617,6 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -638,33 +629,37 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -677,6 +672,9 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -704,10 +702,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="20 % - Accent1" xfId="2" builtinId="30"/>
@@ -843,7 +837,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$T$6:$T$18</c:f>
+              <c:f>Feuil1!$M$6:$M$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -891,7 +885,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$U$6:$U$18</c:f>
+              <c:f>Feuil1!$N$6:$N$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -972,7 +966,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$W$6:$W$18</c:f>
+              <c:f>Feuil1!$P$6:$P$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1020,7 +1014,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$X$6:$X$18</c:f>
+              <c:f>Feuil1!$Q$6:$Q$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1101,7 +1095,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$Z$6:$Z$18</c:f>
+              <c:f>Feuil1!$S$6:$S$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1149,7 +1143,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$AA$6:$AA$18</c:f>
+              <c:f>Feuil1!$T$6:$T$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1948,8 +1942,8 @@
       <xdr:rowOff>43545</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>40821</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>8218714</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -2236,10 +2230,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AA42"/>
+  <dimension ref="B2:T42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U28" sqref="U28"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2249,249 +2243,245 @@
     <col min="4" max="4" width="11.42578125" customWidth="1"/>
     <col min="5" max="5" width="14.140625" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" customWidth="1"/>
+    <col min="8" max="8" width="128" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:27" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84" t="s">
+    <row r="2" spans="2:20" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="84" t="s">
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-    </row>
-    <row r="3" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="W3" s="99"/>
-      <c r="X3" s="99"/>
-      <c r="Y3" s="99"/>
-    </row>
-    <row r="4" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="I2" s="75"/>
+    </row>
+    <row r="3" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P3" s="74"/>
+      <c r="Q3" s="74"/>
+      <c r="R3" s="74"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="38"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="36"/>
       <c r="F4" s="2"/>
-      <c r="T4" s="97" t="s">
+      <c r="M4" s="97" t="s">
         <v>46</v>
       </c>
-      <c r="U4" s="97"/>
-      <c r="W4" s="97" t="s">
+      <c r="N4" s="97"/>
+      <c r="P4" s="97" t="s">
         <v>48</v>
       </c>
-      <c r="X4" s="97"/>
-      <c r="Z4" s="97" t="s">
+      <c r="Q4" s="97"/>
+      <c r="S4" s="97" t="s">
         <v>49</v>
       </c>
-      <c r="AA4" s="97"/>
-    </row>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="T4" s="97"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="33" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="93">
         <v>0.5</v>
       </c>
       <c r="E5" s="94"/>
-      <c r="F5" s="52" t="s">
+      <c r="F5" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="R5" t="s">
+      <c r="K5" t="s">
         <v>47</v>
       </c>
-      <c r="T5" t="s">
+      <c r="M5" t="s">
         <v>45</v>
       </c>
-      <c r="U5" t="s">
+      <c r="N5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="98" t="s">
+      <c r="C6" s="73" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="93">
         <v>0</v>
       </c>
       <c r="E6" s="94"/>
-      <c r="F6" s="52" t="s">
+      <c r="F6" s="50" t="s">
         <v>31</v>
       </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <f>J6*(2*PI())/12</f>
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <f>(COS(K6)*$D$19)+$D$18</f>
+        <v>25000</v>
+      </c>
+      <c r="N6">
+        <f>(SIN(K6)*$D$19)+$E$18</f>
+        <v>7500</v>
+      </c>
+      <c r="P6">
+        <f>(COS(K6)*$D$28)+$D$27</f>
+        <v>-16500</v>
+      </c>
       <c r="Q6">
+        <f>(SIN(K6)*$D$28)+$E$27</f>
+        <v>10000</v>
+      </c>
+      <c r="S6">
+        <f>(COS(K6)*$D$37)+$D$36</f>
         <v>0</v>
       </c>
-      <c r="R6">
-        <f>Q6*(2*PI())/12</f>
-        <v>0</v>
-      </c>
       <c r="T6">
-        <f>(COS(R6)*$D$19)+$D$18</f>
-        <v>25000</v>
-      </c>
-      <c r="U6">
-        <f>(SIN(R6)*$D$19)+$E$18</f>
-        <v>7500</v>
-      </c>
-      <c r="W6">
-        <f>(COS(R6)*$D$28)+$D$27</f>
-        <v>-16500</v>
-      </c>
-      <c r="X6">
-        <f>(SIN(R6)*$D$28)+$E$27</f>
-        <v>10000</v>
-      </c>
-      <c r="Z6">
-        <f>(COS(R6)*$D$37)+$D$36</f>
-        <v>0</v>
-      </c>
-      <c r="AA6">
-        <f>(SIN(R6)*$D$37)+$E$36</f>
+        <f>(SIN(K6)*$D$37)+$E$36</f>
         <v>-15000</v>
       </c>
     </row>
-    <row r="7" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="34" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="95">
         <v>1</v>
       </c>
       <c r="E7" s="96"/>
-      <c r="F7" s="53" t="s">
+      <c r="F7" s="51" t="s">
         <v>32</v>
       </c>
+      <c r="J7">
+        <f>J6+1</f>
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ref="K7:K18" si="0">J7*(2*PI())/12</f>
+        <v>0.52359877559829882</v>
+      </c>
+      <c r="M7">
+        <f t="shared" ref="M7:M18" si="1">(COS(K7)*$D$19)+$D$18</f>
+        <v>24330.127018922194</v>
+      </c>
+      <c r="N7">
+        <f t="shared" ref="N7:N18" si="2">(SIN(K7)*$D$19)+$E$18</f>
+        <v>10000</v>
+      </c>
+      <c r="P7">
+        <f t="shared" ref="P7:P18" si="3">(COS(K7)*$D$28)+$D$27</f>
+        <v>-16968.911086754466</v>
+      </c>
       <c r="Q7">
-        <f>Q6+1</f>
-        <v>1</v>
-      </c>
-      <c r="R7">
-        <f t="shared" ref="R7:R18" si="0">Q7*(2*PI())/12</f>
-        <v>0.52359877559829882</v>
+        <f t="shared" ref="Q7:Q18" si="4">(SIN(K7)*$D$28)+$E$27</f>
+        <v>11750</v>
+      </c>
+      <c r="S7">
+        <f t="shared" ref="S7:S18" si="5">(COS(K7)*$D$37)+$D$36</f>
+        <v>-669.8729810778068</v>
       </c>
       <c r="T7">
-        <f t="shared" ref="T7:T18" si="1">(COS(R7)*$D$19)+$D$18</f>
-        <v>24330.127018922194</v>
-      </c>
-      <c r="U7">
-        <f t="shared" ref="U7:U18" si="2">(SIN(R7)*$D$19)+$E$18</f>
-        <v>10000</v>
-      </c>
-      <c r="W7">
-        <f t="shared" ref="W7:W18" si="3">(COS(R7)*$D$28)+$D$27</f>
-        <v>-16968.911086754466</v>
-      </c>
-      <c r="X7">
-        <f t="shared" ref="X7:X18" si="4">(SIN(R7)*$D$28)+$E$27</f>
-        <v>11750</v>
-      </c>
-      <c r="Z7">
-        <f t="shared" ref="Z7:Z18" si="5">(COS(R7)*$D$37)+$D$36</f>
-        <v>-669.8729810778068</v>
-      </c>
-      <c r="AA7">
-        <f t="shared" ref="AA7:AA18" si="6">(SIN(R7)*$D$37)+$E$36</f>
+        <f t="shared" ref="T7:T18" si="6">(SIN(K7)*$D$37)+$E$36</f>
         <v>-12500</v>
       </c>
     </row>
-    <row r="8" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
-      <c r="F8" s="49"/>
-      <c r="Q8">
-        <f t="shared" ref="Q8:Q18" si="7">Q7+1</f>
+      <c r="F8" s="47"/>
+      <c r="J8">
+        <f t="shared" ref="J8:J18" si="7">J7+1</f>
         <v>2</v>
       </c>
-      <c r="R8">
+      <c r="K8">
         <f t="shared" si="0"/>
         <v>1.0471975511965976</v>
       </c>
-      <c r="T8">
+      <c r="M8">
         <f t="shared" si="1"/>
         <v>22500</v>
       </c>
-      <c r="U8">
+      <c r="N8">
         <f t="shared" si="2"/>
         <v>11830.127018922194</v>
       </c>
-      <c r="W8">
+      <c r="P8">
         <f t="shared" si="3"/>
         <v>-18250</v>
       </c>
-      <c r="X8">
+      <c r="Q8">
         <f t="shared" si="4"/>
         <v>13031.088913245534</v>
       </c>
-      <c r="Z8">
+      <c r="S8">
         <f t="shared" si="5"/>
         <v>-2499.9999999999995</v>
       </c>
-      <c r="AA8">
+      <c r="T8">
         <f t="shared" si="6"/>
         <v>-10669.872981077806</v>
       </c>
     </row>
-    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="54"/>
-      <c r="Q9">
+      <c r="E9" s="29"/>
+      <c r="F9" s="52"/>
+      <c r="J9">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="R9">
+      <c r="K9">
         <f t="shared" si="0"/>
         <v>1.5707963267948966</v>
       </c>
-      <c r="T9">
+      <c r="M9">
         <f t="shared" si="1"/>
         <v>20000</v>
       </c>
-      <c r="U9">
+      <c r="N9">
         <f t="shared" si="2"/>
         <v>12500</v>
       </c>
-      <c r="W9">
+      <c r="P9">
         <f t="shared" si="3"/>
         <v>-20000</v>
       </c>
-      <c r="X9">
+      <c r="Q9">
         <f t="shared" si="4"/>
         <v>13500</v>
       </c>
-      <c r="Z9">
+      <c r="S9">
         <f t="shared" si="5"/>
         <v>-5000</v>
       </c>
-      <c r="AA9">
+      <c r="T9">
         <f t="shared" si="6"/>
         <v>-10000</v>
       </c>
     </row>
-    <row r="10" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>6</v>
       </c>
@@ -2502,43 +2492,43 @@
         <v>1</v>
       </c>
       <c r="E10" s="90"/>
-      <c r="F10" s="66" t="s">
+      <c r="F10" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="Q10">
+      <c r="J10">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="R10">
+      <c r="K10">
         <f t="shared" si="0"/>
         <v>2.0943951023931953</v>
       </c>
-      <c r="T10">
+      <c r="M10">
         <f t="shared" si="1"/>
         <v>17500</v>
       </c>
-      <c r="U10">
+      <c r="N10">
         <f t="shared" si="2"/>
         <v>11830.127018922194</v>
       </c>
-      <c r="W10">
+      <c r="P10">
         <f t="shared" si="3"/>
         <v>-21750</v>
       </c>
-      <c r="X10">
+      <c r="Q10">
         <f t="shared" si="4"/>
         <v>13031.088913245536</v>
       </c>
-      <c r="Z10">
+      <c r="S10">
         <f t="shared" si="5"/>
         <v>-7499.9999999999991</v>
       </c>
-      <c r="AA10">
+      <c r="T10">
         <f t="shared" si="6"/>
         <v>-10669.872981077806</v>
       </c>
     </row>
-    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>7</v>
       </c>
@@ -2551,43 +2541,43 @@
       <c r="E11" s="17">
         <v>0</v>
       </c>
-      <c r="F11" s="50" t="s">
+      <c r="F11" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="Q11">
+      <c r="J11">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="R11">
+      <c r="K11">
         <f t="shared" si="0"/>
         <v>2.6179938779914944</v>
       </c>
-      <c r="T11">
+      <c r="M11">
         <f t="shared" si="1"/>
         <v>15669.872981077806</v>
       </c>
-      <c r="U11">
+      <c r="N11">
         <f t="shared" si="2"/>
         <v>10000</v>
       </c>
-      <c r="W11">
+      <c r="P11">
         <f t="shared" si="3"/>
         <v>-23031.088913245534</v>
       </c>
-      <c r="X11">
+      <c r="Q11">
         <f t="shared" si="4"/>
         <v>11750</v>
       </c>
-      <c r="Z11">
+      <c r="S11">
         <f t="shared" si="5"/>
         <v>-9330.1270189221941</v>
       </c>
-      <c r="AA11">
+      <c r="T11">
         <f t="shared" si="6"/>
         <v>-12500</v>
       </c>
     </row>
-    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>8</v>
       </c>
@@ -2600,43 +2590,43 @@
       <c r="E12" s="17">
         <v>0</v>
       </c>
-      <c r="F12" s="50" t="s">
+      <c r="F12" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="Q12">
+      <c r="J12">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
-      <c r="R12">
+      <c r="K12">
         <f t="shared" si="0"/>
         <v>3.1415926535897931</v>
       </c>
-      <c r="T12">
+      <c r="M12">
         <f t="shared" si="1"/>
         <v>15000</v>
       </c>
-      <c r="U12">
+      <c r="N12">
         <f t="shared" si="2"/>
         <v>7500.0000000000009</v>
       </c>
-      <c r="W12">
+      <c r="P12">
         <f t="shared" si="3"/>
         <v>-23500</v>
       </c>
-      <c r="X12">
+      <c r="Q12">
         <f t="shared" si="4"/>
         <v>10000</v>
       </c>
-      <c r="Z12">
+      <c r="S12">
         <f t="shared" si="5"/>
         <v>-10000</v>
       </c>
-      <c r="AA12">
+      <c r="T12">
         <f t="shared" si="6"/>
         <v>-15000</v>
       </c>
     </row>
-    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>9</v>
       </c>
@@ -2649,43 +2639,43 @@
       <c r="E13" s="17">
         <v>0</v>
       </c>
-      <c r="F13" s="50" t="s">
+      <c r="F13" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="Q13">
+      <c r="J13">
         <f t="shared" si="7"/>
         <v>7</v>
       </c>
-      <c r="R13">
+      <c r="K13">
         <f t="shared" si="0"/>
         <v>3.6651914291880918</v>
       </c>
-      <c r="T13">
+      <c r="M13">
         <f t="shared" si="1"/>
         <v>15669.872981077806</v>
       </c>
-      <c r="U13">
+      <c r="N13">
         <f t="shared" si="2"/>
         <v>5000.0000000000018</v>
       </c>
-      <c r="W13">
+      <c r="P13">
         <f t="shared" si="3"/>
         <v>-23031.088913245534</v>
       </c>
-      <c r="X13">
+      <c r="Q13">
         <f t="shared" si="4"/>
         <v>8250</v>
       </c>
-      <c r="Z13">
+      <c r="S13">
         <f t="shared" si="5"/>
         <v>-9330.1270189221941</v>
       </c>
-      <c r="AA13">
+      <c r="T13">
         <f t="shared" si="6"/>
         <v>-17500</v>
       </c>
     </row>
-    <row r="14" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="8" t="s">
         <v>10</v>
       </c>
@@ -2696,310 +2686,319 @@
         <v>2500</v>
       </c>
       <c r="E14" s="92"/>
-      <c r="F14" s="51" t="s">
+      <c r="F14" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="Q14">
+      <c r="J14">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="R14">
+      <c r="K14">
         <f t="shared" si="0"/>
         <v>4.1887902047863905</v>
       </c>
-      <c r="T14">
+      <c r="M14">
         <f t="shared" si="1"/>
         <v>17499.999999999996</v>
       </c>
-      <c r="U14">
+      <c r="N14">
         <f t="shared" si="2"/>
         <v>3169.8729810778077</v>
       </c>
-      <c r="W14">
+      <c r="P14">
         <f t="shared" si="3"/>
         <v>-21750</v>
       </c>
-      <c r="X14">
+      <c r="Q14">
         <f t="shared" si="4"/>
         <v>6968.9110867544659</v>
       </c>
-      <c r="Z14">
+      <c r="S14">
         <f t="shared" si="5"/>
         <v>-7500.0000000000018</v>
       </c>
-      <c r="AA14">
+      <c r="T14">
         <f t="shared" si="6"/>
         <v>-19330.12701892219</v>
       </c>
     </row>
-    <row r="15" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="1"/>
-      <c r="F15" s="49"/>
-      <c r="Q15">
+      <c r="F15" s="47"/>
+      <c r="J15">
         <f t="shared" si="7"/>
         <v>9</v>
       </c>
-      <c r="R15">
+      <c r="K15">
         <f t="shared" si="0"/>
         <v>4.7123889803846897</v>
       </c>
-      <c r="T15">
+      <c r="M15">
         <f t="shared" si="1"/>
         <v>20000</v>
       </c>
-      <c r="U15">
+      <c r="N15">
         <f t="shared" si="2"/>
         <v>2500</v>
       </c>
-      <c r="W15">
+      <c r="P15">
         <f t="shared" si="3"/>
         <v>-20000</v>
       </c>
-      <c r="X15">
+      <c r="Q15">
         <f t="shared" si="4"/>
         <v>6500</v>
       </c>
-      <c r="Z15">
+      <c r="S15">
         <f t="shared" si="5"/>
         <v>-5000.0000000000009</v>
       </c>
-      <c r="AA15">
+      <c r="T15">
         <f t="shared" si="6"/>
         <v>-20000</v>
       </c>
     </row>
-    <row r="16" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="33" t="s">
+    <row r="16" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="55"/>
-      <c r="Q16">
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="53"/>
+      <c r="J16">
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
-      <c r="R16">
+      <c r="K16">
         <f t="shared" si="0"/>
         <v>5.2359877559829888</v>
       </c>
-      <c r="T16">
+      <c r="M16">
         <f t="shared" si="1"/>
         <v>22500</v>
       </c>
-      <c r="U16">
+      <c r="N16">
         <f t="shared" si="2"/>
         <v>3169.8729810778068</v>
       </c>
-      <c r="W16">
+      <c r="P16">
         <f t="shared" si="3"/>
         <v>-18250</v>
       </c>
-      <c r="X16">
+      <c r="Q16">
         <f t="shared" si="4"/>
         <v>6968.911086754465</v>
       </c>
-      <c r="Z16">
+      <c r="S16">
         <f t="shared" si="5"/>
         <v>-2499.9999999999995</v>
       </c>
-      <c r="AA16">
+      <c r="T16">
         <f t="shared" si="6"/>
         <v>-19330.127018922194</v>
       </c>
     </row>
-    <row r="17" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B17" s="27" t="s">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B17" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="11"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="56"/>
-      <c r="Q17">
+      <c r="D17" s="68"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="54"/>
+      <c r="J17">
         <f t="shared" si="7"/>
         <v>11</v>
       </c>
-      <c r="R17">
+      <c r="K17">
         <f t="shared" si="0"/>
         <v>5.7595865315812871</v>
       </c>
-      <c r="T17">
+      <c r="M17">
         <f t="shared" si="1"/>
         <v>24330.12701892219</v>
       </c>
-      <c r="U17">
+      <c r="N17">
         <f t="shared" si="2"/>
         <v>4999.9999999999982</v>
       </c>
-      <c r="W17">
+      <c r="P17">
         <f t="shared" si="3"/>
         <v>-16968.911086754466</v>
       </c>
-      <c r="X17">
+      <c r="Q17">
         <f t="shared" si="4"/>
         <v>8249.9999999999982</v>
       </c>
-      <c r="Z17">
+      <c r="S17">
         <f t="shared" si="5"/>
         <v>-669.87298107780771</v>
       </c>
-      <c r="AA17">
+      <c r="T17">
         <f t="shared" si="6"/>
         <v>-17500.000000000004</v>
       </c>
     </row>
-    <row r="18" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B18" s="28" t="s">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B18" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="74" t="s">
+      <c r="C18" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="72">
+      <c r="D18" s="69">
         <v>20000</v>
       </c>
-      <c r="E18" s="73">
+      <c r="E18" s="70">
         <v>7500</v>
       </c>
-      <c r="F18" s="69" t="s">
+      <c r="F18" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="Q18">
+      <c r="J18">
         <f t="shared" si="7"/>
         <v>12</v>
       </c>
-      <c r="R18">
+      <c r="K18">
         <f t="shared" si="0"/>
         <v>6.2831853071795862</v>
       </c>
-      <c r="T18">
+      <c r="M18">
         <f t="shared" si="1"/>
         <v>25000</v>
       </c>
-      <c r="U18">
+      <c r="N18">
         <f t="shared" si="2"/>
         <v>7499.9999999999991</v>
       </c>
-      <c r="W18">
+      <c r="P18">
         <f t="shared" si="3"/>
         <v>-16500</v>
       </c>
-      <c r="X18">
+      <c r="Q18">
         <f t="shared" si="4"/>
         <v>10000</v>
       </c>
-      <c r="Z18">
+      <c r="S18">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AA18">
+      <c r="T18">
         <f t="shared" si="6"/>
         <v>-15000.000000000002</v>
       </c>
     </row>
-    <row r="19" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B19" s="28" t="s">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B19" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="74" t="s">
+      <c r="C19" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="85">
+      <c r="D19" s="84">
         <v>5000</v>
       </c>
-      <c r="E19" s="86"/>
-      <c r="F19" s="69" t="s">
+      <c r="E19" s="85"/>
+      <c r="F19" s="67" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B20" s="28" t="s">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B20" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="74" t="s">
+      <c r="C20" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="85">
+      <c r="D20" s="84">
         <v>1</v>
       </c>
-      <c r="E20" s="86"/>
-      <c r="F20" s="69" t="s">
+      <c r="E20" s="85"/>
+      <c r="F20" s="67" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B21" s="28" t="s">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="74" t="s">
+      <c r="C21" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="71"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="69" t="s">
+      <c r="D21" s="84">
+        <f>(4*PI()*POWER(D19,3))/3</f>
+        <v>523598775598.29883</v>
+      </c>
+      <c r="E21" s="85"/>
+      <c r="F21" s="67" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B22" s="28" t="s">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B22" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="74" t="s">
+      <c r="C22" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="71"/>
-      <c r="E22" s="71"/>
-      <c r="F22" s="69" t="s">
+      <c r="D22" s="84">
+        <f>D21*D20</f>
+        <v>523598775598.29883</v>
+      </c>
+      <c r="E22" s="85"/>
+      <c r="F22" s="67" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B23" s="28" t="s">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B23" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="74" t="s">
+      <c r="C23" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="71"/>
-      <c r="E23" s="71"/>
-      <c r="F23" s="69" t="s">
+      <c r="D23" s="84">
+        <f>D19*D7</f>
+        <v>5000</v>
+      </c>
+      <c r="E23" s="85"/>
+      <c r="F23" s="67" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="32" t="s">
+    <row r="24" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="75" t="s">
+      <c r="C24" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="87" t="s">
+      <c r="D24" s="86" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="88"/>
-      <c r="F24" s="68" t="s">
+      <c r="E24" s="87"/>
+      <c r="F24" s="66" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="29"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="57"/>
-    </row>
-    <row r="26" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B26" s="39" t="s">
+    <row r="25" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="27"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="55"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="58"/>
-    </row>
-    <row r="27" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="C26" s="39"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="56"/>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>13</v>
       </c>
@@ -3009,14 +3008,14 @@
       <c r="D27" s="20">
         <v>-20000</v>
       </c>
-      <c r="E27" s="22">
+      <c r="E27" s="21">
         <v>10000</v>
       </c>
-      <c r="F27" s="59" t="s">
+      <c r="F27" s="57" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>14</v>
       </c>
@@ -3027,11 +3026,11 @@
         <v>3500</v>
       </c>
       <c r="E28" s="77"/>
-      <c r="F28" s="60" t="s">
+      <c r="F28" s="58" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>15</v>
       </c>
@@ -3042,79 +3041,88 @@
         <v>1</v>
       </c>
       <c r="E29" s="77"/>
-      <c r="F29" s="60" t="s">
+      <c r="F29" s="58" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="21"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="60" t="s">
+      <c r="D30" s="76">
+        <f>(4*PI()*POWER(D28,3))/3</f>
+        <v>179594380030.21652</v>
+      </c>
+      <c r="E30" s="77"/>
+      <c r="F30" s="58" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D31" s="21"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="60" t="s">
+      <c r="D31" s="76">
+        <f>D29*D30</f>
+        <v>179594380030.21652</v>
+      </c>
+      <c r="E31" s="77"/>
+      <c r="F31" s="58" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="21"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="60" t="s">
+      <c r="D32" s="76">
+        <f>D28*D7</f>
+        <v>3500</v>
+      </c>
+      <c r="E32" s="77"/>
+      <c r="F32" s="58" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="40" t="s">
+      <c r="B33" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="42" t="s">
+      <c r="C33" s="40" t="s">
         <v>43</v>
       </c>
       <c r="D33" s="78" t="s">
         <v>36</v>
       </c>
       <c r="E33" s="79"/>
-      <c r="F33" s="61" t="s">
+      <c r="F33" s="59" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="34" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="29"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="62"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="60"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="45" t="s">
+      <c r="B35" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="46"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="48"/>
-      <c r="F35" s="63"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="61"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
@@ -3123,13 +3131,13 @@
       <c r="C36" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="24">
+      <c r="D36" s="22">
         <v>-5000</v>
       </c>
-      <c r="E36" s="25">
+      <c r="E36" s="23">
         <v>-15000</v>
       </c>
-      <c r="F36" s="64" t="s">
+      <c r="F36" s="62" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3144,7 +3152,7 @@
         <v>5000</v>
       </c>
       <c r="E37" s="83"/>
-      <c r="F37" s="64" t="s">
+      <c r="F37" s="62" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3159,7 +3167,7 @@
         <v>1</v>
       </c>
       <c r="E38" s="83"/>
-      <c r="F38" s="64" t="s">
+      <c r="F38" s="62" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3170,9 +3178,12 @@
       <c r="C39" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="24"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="64" t="s">
+      <c r="D39" s="82">
+        <f>(4*PI()*POWER(D37,3))/3</f>
+        <v>523598775598.29883</v>
+      </c>
+      <c r="E39" s="83"/>
+      <c r="F39" s="62" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3183,9 +3194,12 @@
       <c r="C40" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D40" s="24"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="64" t="s">
+      <c r="D40" s="82">
+        <f>D39*D38</f>
+        <v>523598775598.29883</v>
+      </c>
+      <c r="E40" s="83"/>
+      <c r="F40" s="62" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3196,9 +3210,12 @@
       <c r="C41" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D41" s="24"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="64" t="s">
+      <c r="D41" s="82">
+        <f>D37*D7</f>
+        <v>5000</v>
+      </c>
+      <c r="E41" s="83"/>
+      <c r="F41" s="62" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3213,31 +3230,39 @@
         <v>36</v>
       </c>
       <c r="E42" s="81"/>
-      <c r="F42" s="65" t="s">
+      <c r="F42" s="63" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="Z4:AA4"/>
+  <mergeCells count="27">
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="S4:T4"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D24:E24"/>
-    <mergeCell ref="H2:O2"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D21:E21"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D32:E32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>